<commit_message>
added BT and WWT, fixed some stuff
</commit_message>
<xml_diff>
--- a/lignin_saf/heat_utilities_summary.xlsx
+++ b/lignin_saf/heat_utilities_summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,10 +467,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>829245098.1993092</v>
+        <v>829300028.4920082</v>
       </c>
       <c r="D2" t="n">
-        <v>3.493738894589601</v>
+        <v>4.57412869797354</v>
       </c>
     </row>
     <row r="3">
@@ -485,10 +485,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>444336958.4562436</v>
+        <v>444337009.392413</v>
       </c>
       <c r="D3" t="n">
-        <v>1.872060886984108</v>
+        <v>2.450807423616483</v>
       </c>
     </row>
     <row r="4">
@@ -506,7 +506,7 @@
         <v>19524356.20021592</v>
       </c>
       <c r="D4" t="n">
-        <v>0.08225915690866221</v>
+        <v>0.107689515177348</v>
       </c>
     </row>
     <row r="5">
@@ -521,10 +521,10 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>10270467.74415829</v>
+        <v>10305322.15321375</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0432710819772243</v>
+        <v>0.05684055008245033</v>
       </c>
     </row>
     <row r="6">
@@ -542,7 +542,7 @@
         <v>2324706.624317655</v>
       </c>
       <c r="D6" t="n">
-        <v>0.009794351476451638</v>
+        <v>0.01282226808070471</v>
       </c>
     </row>
     <row r="7">
@@ -560,7 +560,7 @@
         <v>5975.06979333622</v>
       </c>
       <c r="D7" t="n">
-        <v>2.517390067206501e-05</v>
+        <v>3.29563936755097e-05</v>
       </c>
     </row>
     <row r="8">
@@ -575,10 +575,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>-2019186.584710449</v>
+        <v>-2019186.584710486</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.008507147912909198</v>
+        <v>-0.01113712647578478</v>
       </c>
     </row>
     <row r="9">
@@ -596,7 +596,7 @@
         <v>-9601514.524130747</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.04045267775807818</v>
+        <v>-0.05295859353664479</v>
       </c>
     </row>
     <row r="10">
@@ -611,10 +611,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>-18190636.23184353</v>
+        <v>-18190636.23184341</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.07663998672832373</v>
+        <v>-0.1003331826405141</v>
       </c>
     </row>
     <row r="11">
@@ -632,43 +632,61 @@
         <v>-53349480.82507229</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.224769680965806</v>
+        <v>-0.2942570636440101</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>FLASH107</t>
+          <t>HXN</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Flash</t>
+          <t>HeatExchangerNetwork</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>-323004145.6212597</v>
+        <v>-55986681.98138828</v>
       </c>
       <c r="D12" t="n">
-        <v>-1.36086682830104</v>
+        <v>-0.3088029421885569</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>FLASH107</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Flash</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>-323156771.1969261</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-1.782419643424109</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
           <t>HX115</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t>HXutility</t>
         </is>
       </c>
-      <c r="C13" t="n">
+      <c r="C14" t="n">
         <v>-662190832.0417376</v>
       </c>
-      <c r="D13" t="n">
-        <v>-2.789913224170561</v>
+      <c r="D14" t="n">
+        <v>-3.65241285941458</v>
       </c>
     </row>
   </sheetData>

</xml_diff>